<commit_message>
All the committed functionalities mentioned below.
1. Added few objects in object repository
2. ActionHelper class added
3. One keyword driven test case added.
4. ExcelHelper is modified to point to new keyword test cases.
5. LoginLogout functional library added.
6. Modified read config property to get username and password from
config file.
7. StartWebDriver modified : Made Read config object static to allow
access from helper classes.
8. New test case is added in excel file.
9. Verification helpers methods are added.
10. Config properties modified to give username and password.
11. Few modular test is added in testframework class.
</commit_message>
<xml_diff>
--- a/src/java/tests/keywordtestcases/TestCases.xlsx
+++ b/src/java/tests/keywordtestcases/TestCases.xlsx
@@ -5,14 +5,15 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\1_STUDY\EclipseWorkPlace_New\KeywordDriven_withObjectRepository\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\1_STUDY\EclipseWorkPlace_New\KeywordDriven_withObjectRepository\src\java\tests\keywordtestcases\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="leathershoplogin" sheetId="1" r:id="rId1"/>
+    <sheet name="cangotomensformalshoepage" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="38">
   <si>
     <t>TC_NO</t>
   </si>
@@ -71,9 +72,6 @@
     <t>clickLink</t>
   </si>
   <si>
-    <t>verifyText</t>
-  </si>
-  <si>
     <t>sandipan.mca@gmail.com</t>
   </si>
   <si>
@@ -90,13 +88,64 @@
   </si>
   <si>
     <t>Locator Key</t>
+  </si>
+  <si>
+    <t>verifyExactText</t>
+  </si>
+  <si>
+    <t>Verification Text</t>
+  </si>
+  <si>
+    <t>TC_02</t>
+  </si>
+  <si>
+    <t>Log in to site</t>
+  </si>
+  <si>
+    <t>Move to menu option men</t>
+  </si>
+  <si>
+    <t>leathershop.menu.men</t>
+  </si>
+  <si>
+    <t>moveToElement</t>
+  </si>
+  <si>
+    <t>Move to sub menu formal and click</t>
+  </si>
+  <si>
+    <t>leathershop.men.submenu.formal</t>
+  </si>
+  <si>
+    <t>moveToElementAndClick</t>
+  </si>
+  <si>
+    <t>Vefify formal page</t>
+  </si>
+  <si>
+    <t>leathershop.men.formalshoepage.formaltext</t>
+  </si>
+  <si>
+    <t>verifyTextContains</t>
+  </si>
+  <si>
+    <t>FORMAL</t>
+  </si>
+  <si>
+    <t>Log out from site</t>
+  </si>
+  <si>
+    <t>logoutFromSite</t>
+  </si>
+  <si>
+    <t>loginToSite</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -108,6 +157,14 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -134,9 +191,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -418,21 +476,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="18.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="44.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="24.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -440,7 +499,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D1" t="s">
         <v>2</v>
@@ -448,8 +507,11 @@
       <c r="E1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -463,7 +525,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -474,13 +536,13 @@
         <v>10</v>
       </c>
       <c r="D3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -491,13 +553,13 @@
         <v>11</v>
       </c>
       <c r="D4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -508,10 +570,10 @@
         <v>12</v>
       </c>
       <c r="D5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -522,10 +584,10 @@
         <v>13</v>
       </c>
       <c r="D6" t="s">
-        <v>15</v>
-      </c>
-      <c r="E6" t="s">
-        <v>18</v>
+        <v>21</v>
+      </c>
+      <c r="F6" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -534,4 +596,114 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="42.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C5" t="s">
+        <v>32</v>
+      </c>
+      <c r="D5" t="s">
+        <v>33</v>
+      </c>
+      <c r="F5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" t="s">
+        <v>35</v>
+      </c>
+      <c r="D6" t="s">
+        <v>36</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Fixed the introduced Bug.
</commit_message>
<xml_diff>
--- a/src/java/tests/keywordtestcases/TestCases.xlsx
+++ b/src/java/tests/keywordtestcases/TestCases.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="48">
   <si>
     <t>TC_NO</t>
   </si>
@@ -170,9 +170,6 @@
   </si>
   <si>
     <t>verifyComboSelection</t>
-  </si>
-  <si>
-    <t>Price: Lowest firs</t>
   </si>
 </sst>
 </file>
@@ -832,7 +829,7 @@
         <v>47</v>
       </c>
       <c r="F5" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>